<commit_message>
AMoviePage excel file added
</commit_message>
<xml_diff>
--- a/src/tasks/day2Tasks/BrowseListTestCases.xlsx
+++ b/src/tasks/day2Tasks/BrowseListTestCases.xlsx
@@ -5,20 +5,31 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kseniia\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\13138\Desktop\Selenium\projects\movieO\src\tasks\day2Tasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27CF95D0-4E4E-4267-BDBD-B1E4174CD5F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA342B8-07DD-406B-A587-2AFE63D0A0BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -554,20 +565,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" customWidth="1"/>
-    <col min="3" max="3" width="33.42578125" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+    <col min="3" max="3" width="33.44140625" customWidth="1"/>
     <col min="4" max="4" width="42" customWidth="1"/>
-    <col min="5" max="5" width="72.140625" customWidth="1"/>
+    <col min="5" max="5" width="72.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -585,7 +596,7 @@
       </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -599,8 +610,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:6" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -614,7 +625,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -628,7 +639,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -642,7 +653,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -656,7 +667,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -670,7 +681,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
@@ -684,7 +695,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -698,7 +709,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
@@ -712,7 +723,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
@@ -729,7 +740,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>36</v>
       </c>

</xml_diff>